<commit_message>
fixed some nubers. stats update by 30th June 10:00 UTC
</commit_message>
<xml_diff>
--- a/kvk_start_power.xlsx
+++ b/kvk_start_power.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\py_apps\KD1662_bot\kd1662\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D492965A-B13D-4E72-8EB7-BF515D330AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5C217D-4D32-4D84-80AD-2539E9778DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{1CE57D95-D701-4F06-86EE-D14B8AAA3EAA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{1CE57D95-D701-4F06-86EE-D14B8AAA3EAA}"/>
   </bookViews>
   <sheets>
     <sheet name="2025-05-20" sheetId="1" r:id="rId1"/>
@@ -1301,14 +1301,15 @@
   </sheetPr>
   <dimension ref="A1:P265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="A266" sqref="A266:XFD276"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -2795,7 +2796,7 @@
         <v>49499709</v>
       </c>
       <c r="C31" s="2">
-        <v>755190322</v>
+        <v>75519032</v>
       </c>
       <c r="D31" s="2">
         <v>6004975522</v>

</xml_diff>